<commit_message>
cleaned up regression suites; added ctdc quick run
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyOSA01-Biobank_SampleSite_SampleType.xlsx
+++ b/InputFiles/TC01_Canine_StudyOSA01-Biobank_SampleSite_SampleType.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Develope_2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D951BA-4AA3-4269-AC1A-24B82C1BB7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742E58F9-27A1-4F61-B856-680226A2BB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -63,26 +63,6 @@
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c), (samp:sample)--&gt;(c)
 WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and
 samp.summarized_sample_type IN ['Whole Blood']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c), (samp:sample)--&gt;(c)
-WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and
-samp.summarized_sample_type IN ['Whole Blood']
 WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
@@ -98,40 +78,6 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis) ,(r:registration)--&gt;(c), (samp:sample)--&gt;(c)
-WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and
-samp.summarized_sample_type IN ['Whole Blood']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis),(r:registration)--&gt;(c), (samp:sample)--&gt;(c)
-WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and
-samp.summarized_sample_type IN ['Whole Blood']
-WITH DISTINCT f, s
-RETURN 
-  coalesce(f.file_name, '') AS `File Name`,
-  coalesce(f.file_type, '') AS `File Type`,
-  coalesce("study", '') AS `Association`,
-  coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS `File Format`,
-  coalesce(f.file_size, '') AS `Size`,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
     <t>TC01_Canine_StudyOSA01-Biobank_SampleSite_SampleType_Neo4jData.xlsx</t>
   </si>
   <si>
@@ -151,6 +97,88 @@
 count(distinct samp) AS Samples,
 count(distinct f) AS `Case Files`,
 count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c), (samp:sample)--&gt;(c)
+WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and
+samp.summarized_sample_type IN ['Whole Blood']OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis) ,(r:registration)--&gt;(c), (samp:sample)--&gt;(c)
+WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and samp.summarized_sample_type IN ['Whole Blood']
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp:sample)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis),(r:registration)--&gt;(c), (samp:sample)--&gt;(c)
+WHERE samp.sample_site = "Blood" and s.clinical_study_designation IN ['OSA01'] and r.registration_origin in ['CCOGC'] and samp.summarized_sample_type IN ['Whole Blood']
+WITH DISTINCT f,  s, c, demo, diag
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH    
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH    
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+</t>
   </si>
 </sst>
 </file>
@@ -531,7 +559,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="56.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -572,16 +600,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -589,16 +617,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -606,16 +634,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -623,16 +651,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="273" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>